<commit_message>
Updated tensor, letT terms and corresponding printers
</commit_message>
<xml_diff>
--- a/time-labor/week-of-18july2016.xlsx
+++ b/time-labor/week-of-18july2016.xlsx
@@ -61,6 +61,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -150,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0800 – 1000, 1200 – 1400</t>
   </si>
   <si>
     <t xml:space="preserve">Wednesday</t>
@@ -633,13 +637,13 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -880,13 +884,17 @@
       <c r="B14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="D14" s="20" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21" t="n">
         <f aca="false">IF((((D14-C14)+(F14-E14))*24)&gt;8,8,((D14-C14)+(F14-E14))*24)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="21" t="n">
         <f aca="false">IF(((D14-C14)+(F14-E14))*24&gt;8,((D14-C14)+(F14-E14))*24-8,0)</f>
@@ -895,14 +903,16 @@
       <c r="I14" s="22"/>
       <c r="J14" s="23"/>
       <c r="K14" s="24"/>
-      <c r="L14" s="0"/>
+      <c r="L14" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="0"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
@@ -920,7 +930,7 @@
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -941,7 +951,7 @@
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
@@ -961,7 +971,7 @@
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -981,7 +991,7 @@
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
@@ -1005,11 +1015,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1031,7 +1041,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1053,7 +1063,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1069,7 +1079,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1098,14 +1108,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1118,14 +1128,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1165,7 @@
     <mergeCell ref="F26:I26"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F19" type="time">
+    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F14 C15:C19 E15:F15 D16:F19" type="time">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Added top-level Let expression for REPL
</commit_message>
<xml_diff>
--- a/time-labor/week-of-18july2016.xlsx
+++ b/time-labor/week-of-18july2016.xlsx
@@ -65,6 +65,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -172,6 +173,9 @@
   </si>
   <si>
     <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0900 – 1000, 1300 – 1500</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
@@ -646,7 +650,7 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -973,12 +977,17 @@
       <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="0"/>
+      <c r="C17" s="19" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
-        <v>0</v>
+        <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
+        <v>3</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -987,11 +996,13 @@
       <c r="I17" s="22"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="0"/>
+      <c r="L17" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -1011,7 +1022,7 @@
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
@@ -1035,11 +1046,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1061,7 +1072,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1083,7 +1094,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1099,7 +1110,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>170</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1128,14 +1139,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1148,14 +1159,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1196,7 @@
     <mergeCell ref="F26:I26"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F16 C17:C19 E17:F17 D18:F19" type="time">
+    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F19" type="time">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>